<commit_message>
SAdded ContextualQuestionAlgorithm.py, MentalProfile.py, RecommendationAlgorithm.py
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -5,17 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L\PycharmProjects\Testproject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L\PycharmProjects\MentalHealthApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A9E6C1-13DB-4BDD-B088-04FB3611DB78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408408C3-088E-4DB5-AD15-5743C00FB6A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1" sheetId="1" r:id="rId1"/>
     <sheet name="Backend" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -533,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -863,16 +862,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8471D4A-9B34-43C4-BCC1-079161ED168B}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>